<commit_message>
Revert "Control Unit's Changes"
This reverts commit 05ac3801eebe45a8d0d9f27883d11aeae65e63ec.
</commit_message>
<xml_diff>
--- a/module-3/instructions.xlsx
+++ b/module-3/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\METU-NCC-Computer-Architecture\documents\module-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad Yousaf\Desktop\METU NCC\Courses\EEE 446\Lab\Lab 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579B3718-C4EC-45B4-BE3D-1CA537E6011D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39EAD19-FC1C-49EF-A0E2-1D944771F780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,15 +392,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,12 +410,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -672,7 +659,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -722,7 +709,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -762,7 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1167,21 +1152,21 @@
       <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="15" width="18.42578125" customWidth="1"/>
+    <col min="1" max="15" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -1198,7 +1183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1215,17 +1200,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    <row r="4" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1235,12 +1220,12 @@
       <c r="C6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>6</v>
       </c>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1250,48 +1235,48 @@
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>4</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>12</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-    </row>
-    <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B11:E11"/>
@@ -1309,24 +1294,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44D080D-8FD1-4A09-A541-CF81D00D5AF8}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="76.77734375" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
@@ -1349,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -1371,9 +1356,8 @@
       <c r="G2" s="8">
         <v>0</v>
       </c>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1395,9 +1379,8 @@
       <c r="G3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -1419,9 +1402,8 @@
       <c r="G4" s="8">
         <v>1</v>
       </c>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -1443,9 +1425,8 @@
       <c r="G5" s="8">
         <v>4</v>
       </c>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1467,9 +1448,8 @@
       <c r="G6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1491,9 +1471,8 @@
       <c r="G7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>91</v>
       </c>
@@ -1516,7 +1495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1538,9 +1517,8 @@
       <c r="G9" s="8">
         <v>6</v>
       </c>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>75</v>
       </c>
@@ -1562,9 +1540,8 @@
       <c r="G10" s="8">
         <v>5</v>
       </c>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
@@ -1586,9 +1563,8 @@
       <c r="G11" s="8">
         <v>2</v>
       </c>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -1610,9 +1586,8 @@
       <c r="G12" s="8">
         <v>7</v>
       </c>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -1634,9 +1609,8 @@
       <c r="G13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1658,9 +1632,8 @@
       <c r="G14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -1682,9 +1655,8 @@
       <c r="G15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>69</v>
       </c>
@@ -1706,9 +1678,8 @@
       <c r="G16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>71</v>
       </c>
@@ -1730,9 +1701,8 @@
       <c r="G17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>72</v>
       </c>
@@ -1754,9 +1724,8 @@
       <c r="G18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>70</v>
       </c>
@@ -1778,9 +1747,8 @@
       <c r="G19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>73</v>
       </c>
@@ -1802,9 +1770,8 @@
       <c r="G20" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>74</v>
       </c>
@@ -1826,9 +1793,8 @@
       <c r="G21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -1851,7 +1817,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>22</v>
       </c>
@@ -1874,7 +1840,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
@@ -1897,7 +1863,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>

</xml_diff>